<commit_message>
Finish dropdowns, start on raw data download option
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_HTML5\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833A429D-09A1-4D08-AC95-604830F1F48E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C363317-A481-4BDB-806E-B0C0A473F376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16395" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="1380" windowWidth="27930" windowHeight="13830" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="4.9" sheetId="9" r:id="rId1"/>
+    <sheet name="bugs" sheetId="9" r:id="rId1"/>
     <sheet name="Sue Saupe concerns" sheetId="8" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
     <sheet name="layers show issue" sheetId="7" r:id="rId4"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -330,25 +330,72 @@
     <t>Steve will do?</t>
   </si>
   <si>
-    <t>[esri.views.LayerViewFactory] Failed to create view for layer 'Terrain3D, id:worldElevation' of type 'elevation'. Object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  b._consoleWriter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  b.log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  b.error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (anonymous function)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  a</t>
-  </si>
-  <si>
-    <t>Version 4.9 gives this error, after"ExpandoPane…" and "MapStuff object created":</t>
+    <r>
+      <t xml:space="preserve">interaction between </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regions/Sites</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Species</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> table </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dropdowns</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -679,7 +726,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1014,50 +1061,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8762A0-C6E1-4E4F-887F-5F4A028E733F}">
-  <dimension ref="A3:A9"/>
+  <dimension ref="A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.25" style="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misc. bug fixes & modifications
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF55F08-24F1-41A8-BBAA-77B1BCFC6027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF068DF6-DF9F-47B2-B639-4839AAE23619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="1350" windowWidth="28290" windowHeight="13830" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="330" yWindow="1305" windowWidth="28290" windowHeight="13830" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bugs" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -338,6 +338,12 @@
   <si>
     <t>Eventually get the dropdowns to respond to spatial filter as well?</t>
   </si>
+  <si>
+    <t>Cancel button for Species dropdown panel</t>
+  </si>
+  <si>
+    <t>File name should be "Fish Catch for Alaska"?</t>
+  </si>
 </sst>
 </file>
 
@@ -530,7 +536,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,6 +546,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -587,7 +599,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -659,6 +671,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,9 +683,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -694,6 +708,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3247634</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152264</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBF4B385-3B92-40B0-9568-C50D486C61BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="1266825"/>
+          <a:ext cx="3123809" cy="1085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1005,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8762A0-C6E1-4E4F-887F-5F4A028E733F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1027,13 +1090,42 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="37" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1396,13 +1488,13 @@
   <sheetData>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -1593,7 +1685,7 @@
       <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="39" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -1601,7 +1693,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
@@ -1641,7 +1733,7 @@
       <c r="C20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="40" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1649,7 +1741,7 @@
       <c r="C21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="39"/>
+      <c r="E21" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Misc. changes & bug fixes
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4E0108-349C-44C7-8FB7-E7351CB6E7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEAEBC7-58EF-421F-8F02-D34081F6CFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1170" windowWidth="28290" windowHeight="13830" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="2085" windowWidth="24285" windowHeight="13260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FA bugs" sheetId="9" r:id="rId1"/>
@@ -22,11 +22,21 @@
     <sheet name="questions" sheetId="3" r:id="rId7"/>
     <sheet name="API wish list" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,7 +51,7 @@
     <author>Jim</author>
   </authors>
   <commentList>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
+    <comment ref="A39" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
       <text>
         <r>
           <rPr>
@@ -70,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -468,12 +478,39 @@
       <t xml:space="preserve"> values so they sort correctly</t>
     </r>
   </si>
+  <si>
+    <t>Photos not coming up</t>
+  </si>
+  <si>
+    <t>FMP filter option not working</t>
+  </si>
+  <si>
+    <t>need field name in vw_FishCounts_flat</t>
+  </si>
+  <si>
+    <t>Also, waiting on new list, possibly with different field name</t>
+  </si>
+  <si>
+    <t>Finish download headers</t>
+  </si>
+  <si>
+    <t>selection box issues</t>
+  </si>
+  <si>
+    <t>change the word Hauls to Sets in the Regions table, Sites table, and Sites popup</t>
+  </si>
+  <si>
+    <t>If a species is currently selected and SP panel is opened again, "Close" button has changed to "Go".  Still works to close panel, though.</t>
+  </si>
+  <si>
+    <t>Put graphic object ID in hidden column?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="34">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -705,6 +742,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -770,7 +828,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -868,6 +926,24 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -877,22 +953,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -923,13 +1003,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3247634</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>152264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1278,11 +1358,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8762A0-C6E1-4E4F-887F-5F4A028E733F}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="A17:C17"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1311,114 +1391,215 @@
       </c>
       <c r="F1" s="38"/>
     </row>
-    <row r="3" spans="1:6" ht="33">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="55"/>
+    </row>
+    <row r="5" spans="1:6" ht="16.5">
+      <c r="A5" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="E5" s="46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5">
-      <c r="A5" s="40" t="s">
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="49" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="43"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="43"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="43"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="43"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="43"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="43"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="31.5">
-      <c r="A19" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="57">
-      <c r="A21" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="41" t="s">
+      <c r="B20" s="55" t="s">
         <v>96</v>
       </c>
     </row>
+    <row r="21" spans="1:3" ht="31.5">
+      <c r="A21" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="55"/>
+    </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="48"/>
-    </row>
-    <row r="23" spans="1:3" ht="28.5">
-      <c r="A23" s="48" t="s">
-        <v>94</v>
+      <c r="A22" s="54"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="57" t="s">
+        <v>110</v>
       </c>
       <c r="B23" s="41" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="48"/>
-    </row>
-    <row r="25" spans="1:3" ht="28.5">
-      <c r="A25" s="48" t="s">
+      <c r="A24" s="54"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="54"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="54"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="54"/>
+    </row>
+    <row r="29" spans="1:3" ht="28.5">
+      <c r="A29" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B29" s="59" t="s">
         <v>96</v>
       </c>
+      <c r="C29" s="59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.5">
+      <c r="A31" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="45"/>
+    </row>
+    <row r="33" spans="1:3" ht="57">
+      <c r="A33" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="45"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="31.5">
+      <c r="A43" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="43"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="43"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="43"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="43"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="43"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="43"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="44" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B20:B21"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A17" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
+    <hyperlink ref="A41" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
@@ -1786,13 +1967,13 @@
   <sheetData>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="18.75">
       <c r="A3" s="8"/>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="18.75">
       <c r="A4" s="9" t="s">
@@ -1983,7 +2164,7 @@
       <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="52" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -1991,7 +2172,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="46"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
@@ -2031,7 +2212,7 @@
       <c r="C20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="53" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2039,7 +2220,7 @@
       <c r="C21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="47"/>
+      <c r="E21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
searchable DD, popup positioning
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEAEBC7-58EF-421F-8F02-D34081F6CFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E318EEE-45B6-4C12-AA4A-1FC0DB81E880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="2085" windowWidth="24285" windowHeight="13260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1335" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FA bugs" sheetId="9" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <author>Jim</author>
   </authors>
   <commentList>
-    <comment ref="A39" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
+    <comment ref="A57" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="119">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -389,9 +389,6 @@
     <t>File name should be "Fish Catch for Alaska"?</t>
   </si>
   <si>
-    <t>Data update</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -411,45 +408,6 @@
   </si>
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Data_Catch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> -- _041022 version </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Regions_Sites_dn.mdb, that has refined region polygons in the feature class named </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Regions_FishAtlas_dn</t>
-    </r>
-  </si>
-  <si>
-    <t>In SQL Server, but not in published map service yet</t>
   </si>
   <si>
     <t xml:space="preserve">I just discovered that while Items and Catch tallies update in response to the sites that are selected, the Hauls and Species tallies don't change. </t>
@@ -491,12 +449,6 @@
     <t>Also, waiting on new list, possibly with different field name</t>
   </si>
   <si>
-    <t>Finish download headers</t>
-  </si>
-  <si>
-    <t>selection box issues</t>
-  </si>
-  <si>
     <t>change the word Hauls to Sets in the Regions table, Sites table, and Sites popup</t>
   </si>
   <si>
@@ -504,13 +456,55 @@
   </si>
   <si>
     <t>Put graphic object ID in hidden column?</t>
+  </si>
+  <si>
+    <t>Put "Species" label next to SP selection button</t>
+  </si>
+  <si>
+    <t>Finish setting download headers</t>
+  </si>
+  <si>
+    <t>Selection of "All" or "FMP" shows up in button text</t>
+  </si>
+  <si>
+    <t>Checking FMP checkbox filters the table on FMP=1</t>
+  </si>
+  <si>
+    <t>selection box issues -- box showing/not showing at inappropriate times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change messages from red font color to black (e.g., "Download in progress….." message in download window, "Looking for photo points" and "Site photos can be seen….." messages in photo panel, and "Looking for sites" message in table panel. </t>
+  </si>
+  <si>
+    <t>In advance of adding a ShoreStation-like species filter into Fish Atlas, would it be easy to add a search field in the window so that if you want data on capelin you can simply type in capelin rather than having to scroll through the list to find it? Also, might said search tool be able to find walleye pollock if someone were to search for just the word pollock? Likewise, might the search tool be able to bring up both Arctic and Pacific sand lance with a search for sandlance or sand lance? In the event this would be a lot of work, please advise on a timeline for the implementation of a ShoreStation-like species filter</t>
+  </si>
+  <si>
+    <t>Changes to raw download csv fieldnames: change WebSiteLocation display to Location, move RawSite immediately after SiteID, add RawEvent immediately after EventID</t>
+  </si>
+  <si>
+    <t>Highlight Sites on mouseover:  bigger, RGB 74, 241, 242</t>
+  </si>
+  <si>
+    <t>The 2 "Show Popups" boxes work differently</t>
+  </si>
+  <si>
+    <t>Add all 5 FMP fields to raw download list</t>
+  </si>
+  <si>
+    <t>Think about more generic browser tab name, to cover SZ, FA &amp; SS.  Maybe "ShoreZone, Fish Atlas &amp; Shore Stations"?</t>
+  </si>
+  <si>
+    <t>pending approval</t>
+  </si>
+  <si>
+    <t>Popups docked by default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -703,19 +697,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -744,14 +725,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
@@ -763,6 +736,14 @@
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -828,7 +809,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -929,20 +910,51 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -953,27 +965,32 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1003,13 +1020,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3247634</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>152264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1358,248 +1375,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8762A0-C6E1-4E4F-887F-5F4A028E733F}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="94.625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="97.125" style="40" customWidth="1"/>
     <col min="2" max="2" width="7.125" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="41"/>
+    <col min="3" max="3" width="9" style="68"/>
     <col min="4" max="4" width="8.875" style="36"/>
-    <col min="5" max="5" width="58.625" style="42" customWidth="1"/>
-    <col min="6" max="6" width="25.125" style="41" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="36"/>
+    <col min="5" max="5" width="25.125" style="41" customWidth="1"/>
+    <col min="6" max="16384" width="8.875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="37" customFormat="1">
+    <row r="1" spans="1:5" s="37" customFormat="1">
       <c r="A1" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B1" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="38"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="55"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5">
-      <c r="A5" s="54" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="E5" s="46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="41" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="31.5">
+      <c r="A11" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="55"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="55"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="42"/>
+      <c r="B12" s="55"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="55"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="55"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="55"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="55"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="55"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="42"/>
+      <c r="B15" s="55"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="55"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="55"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="55"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="36"/>
+      <c r="B17" s="55"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="55"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="36"/>
+      <c r="B18" s="55"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="55"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="36"/>
+      <c r="B19" s="55"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="55"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="36"/>
+      <c r="B20" s="55"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="55"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="36"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="31.5">
+      <c r="A27" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="61"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="49"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="49"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="49"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="49"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="49"/>
+    </row>
+    <row r="35" spans="1:5" s="66" customFormat="1">
+      <c r="A35" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="73"/>
+      <c r="C35" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="65"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="42"/>
+      <c r="B36" s="55"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="55"/>
+    </row>
+    <row r="37" spans="1:5" ht="47.25">
+      <c r="A37" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="56"/>
+      <c r="C37" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="42"/>
+      <c r="E37" s="55"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="42"/>
+      <c r="B38" s="55"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="55"/>
+    </row>
+    <row r="39" spans="1:5" ht="94.5">
+      <c r="A39" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="56"/>
+      <c r="C39" s="69" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="55"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="42"/>
+      <c r="B40" s="55"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="55"/>
+    </row>
+    <row r="41" spans="1:5" ht="21" customHeight="1">
+      <c r="A41" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="56"/>
+      <c r="C41" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="42"/>
+      <c r="E41" s="55"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="36"/>
+      <c r="B42" s="55"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="55"/>
+    </row>
+    <row r="43" spans="1:5" s="57" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A43" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="58"/>
+    </row>
+    <row r="44" spans="1:5" s="57" customFormat="1">
+      <c r="A44" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="60"/>
+      <c r="C44" s="70"/>
+      <c r="E44" s="47"/>
+    </row>
+    <row r="45" spans="1:5" s="57" customFormat="1">
+      <c r="A45" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="60"/>
+      <c r="C45" s="70"/>
+      <c r="E45" s="47"/>
+    </row>
+    <row r="47" spans="1:5" ht="28.5">
+      <c r="A47" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="28.5">
+      <c r="A49" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="45"/>
+    </row>
+    <row r="51" spans="1:3" ht="42.75">
+      <c r="A51" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="45"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="52"/>
+      <c r="C55" s="71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="48" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="40" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="55" t="s">
+      <c r="B59" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="31.5">
+      <c r="A61" s="46" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="31.5">
-      <c r="A21" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" s="55"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="54"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="54"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="54"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="54"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="54"/>
-    </row>
-    <row r="29" spans="1:3" ht="28.5">
-      <c r="A29" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="59" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="28.5">
-      <c r="A31" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="59" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="45"/>
-    </row>
-    <row r="33" spans="1:3" ht="57">
-      <c r="A33" s="61" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="59" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="45"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="59" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="B41" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="49" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="31.5">
-      <c r="A43" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="B43" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="49" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="43"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="43"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="43"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="43"/>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="43"/>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="43"/>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="44" t="s">
+      <c r="B61" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" s="69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="43"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="43"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="43"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="43"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="43"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="43"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="44" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B20:B21"/>
+  <mergeCells count="3">
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C43:C45"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A41" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
+    <hyperlink ref="A59" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
@@ -1967,13 +2133,13 @@
   <sheetData>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="18.75">
       <c r="A3" s="8"/>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="18.75">
       <c r="A4" s="9" t="s">
@@ -2164,7 +2330,7 @@
       <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="63" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -2172,7 +2338,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="52"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
@@ -2212,7 +2378,7 @@
       <c r="C20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="64" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2220,7 +2386,7 @@
       <c r="C21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="53"/>
+      <c r="E21" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Fixed FMP?  Hack to highlight moused-over Site.
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0603D699-87C0-4D9D-A799-E2F62511DCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4B5B99-F481-42D0-AC75-F2A6549872E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1335" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <author>Jim</author>
   </authors>
   <commentList>
-    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
+    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="121">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -502,12 +502,40 @@
   <si>
     <t>"Scientific name" radio button in Species dropdown doesn't work</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">renamed header "Show Popups" to "Show </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Layer</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32">
+  <fonts count="34">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -744,6 +772,23 @@
       <i/>
       <sz val="12"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -812,7 +857,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -986,6 +1031,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1003,6 +1051,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1032,13 +1083,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3247634</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>152264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1387,11 +1438,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8762A0-C6E1-4E4F-887F-5F4A028E733F}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1399,8 +1450,8 @@
     <col min="1" max="1" width="97.125" style="40" customWidth="1"/>
     <col min="2" max="2" width="7.125" style="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="65"/>
-    <col min="4" max="4" width="8.875" style="36"/>
-    <col min="5" max="5" width="25.125" style="41" customWidth="1"/>
+    <col min="4" max="4" width="4.625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="42.75" style="41" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.875" style="36"/>
   </cols>
   <sheetData>
@@ -1451,21 +1502,26 @@
       <c r="E10" s="55"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="71"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="71"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="55"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="42"/>
-      <c r="B12" s="55"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="55"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="78" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="36"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="55"/>
       <c r="D13" s="42"/>
       <c r="E13" s="55"/>
@@ -1488,48 +1544,49 @@
       <c r="D16" s="42"/>
       <c r="E16" s="55"/>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="36" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="36"/>
+      <c r="B17" s="55"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="55"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="36" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="40" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="40" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B23" s="73" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="31.5">
-      <c r="A23" s="49" t="s">
+    <row r="24" spans="1:5" ht="31.5">
+      <c r="A24" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="72"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="49"/>
+      <c r="B24" s="73"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="49"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B26" s="41" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="49"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="49"/>
-      <c r="B27" s="61"/>
-      <c r="E27" s="61"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="49"/>
@@ -1553,33 +1610,27 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="49"/>
+      <c r="B32" s="61"/>
+      <c r="E32" s="61"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="49"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="49"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="60"/>
-      <c r="C34" s="67" t="s">
+      <c r="B35" s="60"/>
+      <c r="C35" s="67" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="31.5">
-      <c r="A36" s="46" t="s">
+    <row r="37" spans="1:5" ht="31.5">
+      <c r="A37" s="46" t="s">
         <v>112</v>
-      </c>
-      <c r="B36" s="60"/>
-      <c r="C36" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="55"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="46" t="s">
-        <v>115</v>
       </c>
       <c r="B37" s="60"/>
       <c r="C37" s="67" t="s">
@@ -1589,200 +1640,208 @@
       <c r="E37" s="55"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="42"/>
-      <c r="B38" s="55"/>
+      <c r="A38" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="60"/>
+      <c r="C38" s="67" t="s">
+        <v>90</v>
+      </c>
       <c r="D38" s="42"/>
       <c r="E38" s="55"/>
     </row>
-    <row r="39" spans="1:5" s="63" customFormat="1">
-      <c r="A39" s="70" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" s="42"/>
+      <c r="B39" s="55"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="55"/>
+    </row>
+    <row r="40" spans="1:5" s="63" customFormat="1">
+      <c r="A40" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="B39" s="69"/>
-      <c r="C39" s="66" t="s">
+      <c r="B40" s="69"/>
+      <c r="C40" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="62"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="42"/>
-      <c r="B40" s="55"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="55"/>
-    </row>
-    <row r="41" spans="1:5" ht="47.25">
-      <c r="A41" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="66" t="s">
-        <v>90</v>
-      </c>
+      <c r="D40" s="62"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="42"/>
+      <c r="B41" s="55"/>
       <c r="D41" s="42"/>
       <c r="E41" s="55"/>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="42"/>
-      <c r="B42" s="55"/>
+    <row r="42" spans="1:5" ht="47.25">
+      <c r="A42" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="66" t="s">
+        <v>90</v>
+      </c>
       <c r="D42" s="42"/>
       <c r="E42" s="55"/>
     </row>
-    <row r="43" spans="1:5" ht="94.5">
-      <c r="A43" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="66" t="s">
-        <v>117</v>
-      </c>
+    <row r="43" spans="1:5">
+      <c r="A43" s="42"/>
+      <c r="B43" s="55"/>
       <c r="D43" s="42"/>
       <c r="E43" s="55"/>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="42"/>
-      <c r="B44" s="55"/>
+    <row r="44" spans="1:5" ht="94.5">
+      <c r="A44" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="56"/>
+      <c r="C44" s="66" t="s">
+        <v>117</v>
+      </c>
       <c r="D44" s="42"/>
       <c r="E44" s="55"/>
     </row>
-    <row r="45" spans="1:5" ht="21" customHeight="1">
-      <c r="A45" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="66" t="s">
-        <v>90</v>
-      </c>
+    <row r="45" spans="1:5">
+      <c r="A45" s="42"/>
+      <c r="B45" s="55"/>
       <c r="D45" s="42"/>
       <c r="E45" s="55"/>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="36"/>
-      <c r="B46" s="55"/>
+    <row r="46" spans="1:5" ht="21" customHeight="1">
+      <c r="A46" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="56"/>
+      <c r="C46" s="66" t="s">
+        <v>90</v>
+      </c>
       <c r="D46" s="42"/>
       <c r="E46" s="55"/>
     </row>
-    <row r="47" spans="1:5" s="57" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A47" s="46" t="s">
+    <row r="47" spans="1:5">
+      <c r="A47" s="36"/>
+      <c r="B47" s="55"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="55"/>
+    </row>
+    <row r="48" spans="1:5" s="57" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A48" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="71" t="s">
+      <c r="B48" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="73" t="s">
+      <c r="C48" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="58"/>
-    </row>
-    <row r="48" spans="1:5" s="57" customFormat="1">
-      <c r="A48" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="71"/>
-      <c r="C48" s="73"/>
-      <c r="E48" s="47"/>
+      <c r="E48" s="58"/>
     </row>
     <row r="49" spans="1:5" s="57" customFormat="1">
       <c r="A49" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="72"/>
+      <c r="C49" s="74"/>
+      <c r="E49" s="47"/>
+    </row>
+    <row r="50" spans="1:5" s="57" customFormat="1">
+      <c r="A50" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="71"/>
-      <c r="C49" s="73"/>
-      <c r="E49" s="47"/>
-    </row>
-    <row r="51" spans="1:5" ht="28.5">
-      <c r="A51" s="54" t="s">
+      <c r="B50" s="72"/>
+      <c r="C50" s="74"/>
+      <c r="E50" s="47"/>
+    </row>
+    <row r="52" spans="1:5" ht="28.5">
+      <c r="A52" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="52" t="s">
+      <c r="B52" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="C51" s="68" t="s">
+      <c r="C52" s="68" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.5">
-      <c r="A53" s="54" t="s">
+    <row r="54" spans="1:5" ht="28.5">
+      <c r="A54" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="B53" s="52" t="s">
+      <c r="B54" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="68" t="s">
+      <c r="C54" s="68" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="45"/>
-    </row>
-    <row r="55" spans="1:5" ht="42.75">
-      <c r="A55" s="54" t="s">
+    <row r="55" spans="1:5">
+      <c r="A55" s="45"/>
+    </row>
+    <row r="56" spans="1:5" ht="42.75">
+      <c r="A56" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="52" t="s">
+      <c r="B56" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="68" t="s">
+      <c r="C56" s="68" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="45"/>
-    </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="45"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="52" t="s">
+      <c r="B58" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="68" t="s">
+      <c r="C58" s="68" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="53" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="52"/>
-      <c r="C59" s="68" t="s">
+      <c r="B60" s="52"/>
+      <c r="C60" s="68" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="46" t="s">
+    <row r="62" spans="1:5">
+      <c r="A62" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="47" t="s">
+      <c r="B62" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="66" t="s">
+      <c r="C62" s="66" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="48" t="s">
+    <row r="64" spans="1:5">
+      <c r="A64" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B63" s="47" t="s">
+      <c r="B64" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C63" s="66" t="s">
+      <c r="C64" s="66" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="31.5">
-      <c r="A65" s="46" t="s">
+    <row r="66" spans="1:3" ht="31.5">
+      <c r="A66" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="B65" s="47" t="s">
+      <c r="B66" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C65" s="66" t="s">
+      <c r="C66" s="66" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="43"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="43"/>
@@ -1800,18 +1859,21 @@
       <c r="A74" s="43"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="44" t="s">
+      <c r="A75" s="43"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="44" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C48:C50"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A63" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
+    <hyperlink ref="A64" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
@@ -2179,13 +2241,13 @@
   <sheetData>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="18.75">
       <c r="A3" s="8"/>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="18.75">
       <c r="A4" s="9" t="s">
@@ -2376,7 +2438,7 @@
       <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="76" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -2384,7 +2446,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="75"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
@@ -2424,7 +2486,7 @@
       <c r="C20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="76" t="s">
+      <c r="E20" s="77" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2432,7 +2494,7 @@
       <c r="C21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="76"/>
+      <c r="E21" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Infrastructure for alternate links (between SZ/FA/SS)
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4B5B99-F481-42D0-AC75-F2A6549872E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A125F99-00DB-4BB9-B6C9-5C46DA2A7279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1335" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1560" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FA bugs" sheetId="9" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="123">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -529,6 +529,12 @@
       </rPr>
       <t>"</t>
     </r>
+  </si>
+  <si>
+    <t>y?</t>
+  </si>
+  <si>
+    <t>Prepare links for switching between SZ/FA/SS</t>
   </si>
 </sst>
 </file>
@@ -1034,6 +1040,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1051,9 +1060,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1442,7 +1448,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1484,140 +1490,153 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="40" t="s">
-        <v>108</v>
-      </c>
+      <c r="A7" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="55"/>
+      <c r="C7" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="40" t="s">
-        <v>107</v>
-      </c>
+      <c r="A8" s="42"/>
+      <c r="B8" s="71"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="71"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="55"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="42" t="s">
-        <v>113</v>
-      </c>
+      <c r="A10" s="36"/>
       <c r="B10" s="55"/>
       <c r="D10" s="42"/>
       <c r="E10" s="55"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="42"/>
-      <c r="B11" s="71"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="55"/>
       <c r="D11" s="42"/>
-      <c r="E11" s="71"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="78" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="42"/>
-      <c r="B13" s="55"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="55"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="55"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="55"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="36"/>
-      <c r="B14" s="55"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="55"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="36"/>
-      <c r="B15" s="55"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="55"/>
+      <c r="A14" s="36" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="36"/>
-      <c r="B16" s="55"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="55"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="36"/>
-      <c r="B17" s="55"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="55"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="36" t="s">
-        <v>119</v>
-      </c>
+      <c r="A16" s="40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="31.5">
+      <c r="A19" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="74"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="49"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="40" t="s">
-        <v>86</v>
-      </c>
+      <c r="A21" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="49"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="73" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="31.5">
-      <c r="A24" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="73"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="61"/>
+      <c r="E23" s="61"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="49"/>
+      <c r="B24" s="61"/>
+      <c r="E24" s="61"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="49"/>
+      <c r="B25" s="61"/>
+      <c r="E25" s="61"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>95</v>
-      </c>
+      <c r="A26" s="49"/>
+      <c r="B26" s="61"/>
+      <c r="E26" s="61"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="49"/>
+      <c r="B27" s="61"/>
+      <c r="E27" s="61"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="49"/>
-      <c r="B28" s="61"/>
-      <c r="E28" s="61"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="49"/>
-      <c r="B29" s="61"/>
-      <c r="E29" s="61"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="49"/>
-      <c r="B30" s="61"/>
-      <c r="E30" s="61"/>
+      <c r="A30" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="52"/>
+      <c r="C30" s="68" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="49"/>
-      <c r="B31" s="61"/>
-      <c r="E31" s="61"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="49"/>
-      <c r="B32" s="61"/>
-      <c r="E32" s="61"/>
+      <c r="A31" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="52"/>
+      <c r="C31" s="68" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="49"/>
+      <c r="A33" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="52"/>
+      <c r="C33" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="51"/>
+      <c r="E33" s="72" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="49"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="55"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="55"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="46" t="s">
@@ -1727,10 +1746,10 @@
       <c r="A48" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="72" t="s">
+      <c r="B48" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="74" t="s">
+      <c r="C48" s="75" t="s">
         <v>90</v>
       </c>
       <c r="E48" s="58"/>
@@ -1739,16 +1758,16 @@
       <c r="A49" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="74"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="75"/>
       <c r="E49" s="47"/>
     </row>
     <row r="50" spans="1:5" s="57" customFormat="1">
       <c r="A50" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="72"/>
-      <c r="C50" s="74"/>
+      <c r="B50" s="73"/>
+      <c r="C50" s="75"/>
       <c r="E50" s="47"/>
     </row>
     <row r="52" spans="1:5" ht="28.5">
@@ -1869,7 +1888,7 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="C48:C50"/>
   </mergeCells>
   <hyperlinks>
@@ -2241,13 +2260,13 @@
   <sheetData>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="18.75">
       <c r="A3" s="8"/>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="18.75">
       <c r="A4" s="9" t="s">
@@ -2438,7 +2457,7 @@
       <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="77" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -2446,7 +2465,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="76"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
@@ -2486,7 +2505,7 @@
       <c r="C20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="78" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2494,7 +2513,7 @@
       <c r="C21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="77"/>
+      <c r="E21" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Cleared up selExtentGraphic issues
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A125F99-00DB-4BB9-B6C9-5C46DA2A7279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31E62A3-43DB-4882-BE72-3A8F4900245B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1560" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -863,7 +863,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1060,6 +1060,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1448,7 +1451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1482,93 +1485,91 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>90</v>
-      </c>
+      <c r="A5" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="55"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="42"/>
+      <c r="B6" s="71"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="71"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="42" t="s">
-        <v>113</v>
-      </c>
+      <c r="A7" s="36"/>
       <c r="B7" s="55"/>
-      <c r="C7" s="65" t="s">
-        <v>121</v>
-      </c>
       <c r="D7" s="42"/>
       <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="42"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="55"/>
       <c r="D8" s="42"/>
-      <c r="E8" s="71"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="55"/>
+      <c r="E8" s="55"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="36"/>
-      <c r="B10" s="55"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="55"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="36"/>
-      <c r="B11" s="55"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="55"/>
+      <c r="A10" s="36" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="36"/>
-      <c r="B12" s="55"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="55"/>
+      <c r="A12" s="40" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="36" t="s">
-        <v>119</v>
-      </c>
+      <c r="A14" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.5">
+      <c r="A15" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="74"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="40" t="s">
-        <v>86</v>
+      <c r="A16" s="49"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="74" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31.5">
-      <c r="A19" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="74"/>
+      <c r="A18" s="49"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="49"/>
+      <c r="B19" s="61"/>
+      <c r="E19" s="61"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="49"/>
+      <c r="B20" s="61"/>
+      <c r="E20" s="61"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>95</v>
-      </c>
+      <c r="A21" s="49"/>
+      <c r="B21" s="61"/>
+      <c r="E21" s="61"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="49"/>
+      <c r="B22" s="61"/>
+      <c r="E22" s="61"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="49"/>
@@ -1577,29 +1578,37 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="49"/>
-      <c r="B24" s="61"/>
-      <c r="E24" s="61"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="49"/>
-      <c r="B25" s="61"/>
-      <c r="E25" s="61"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="49"/>
-      <c r="B26" s="61"/>
-      <c r="E26" s="61"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="49"/>
-      <c r="B27" s="61"/>
-      <c r="E27" s="61"/>
+      <c r="A26" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="68" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="49"/>
+      <c r="A28" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="52"/>
+      <c r="C28" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="42"/>
+      <c r="E28" s="55"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="49"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="55"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="55"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="51" t="s">
@@ -1888,7 +1897,7 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C48:C50"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>

<commit_message>
Spatial filtering on dropdowns, fix FMP & spatial filter info for raw download
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31E62A3-43DB-4882-BE72-3A8F4900245B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74FC77B-31B2-4464-A9F7-A7EEAF17F765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1560" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -1451,7 +1451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1477,79 +1477,81 @@
       <c r="E1" s="38"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>90</v>
-      </c>
+      <c r="A3" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="55"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="42"/>
+      <c r="B4" s="71"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="71"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="68" t="s">
-        <v>121</v>
-      </c>
+      <c r="A5" s="36"/>
+      <c r="B5" s="55"/>
       <c r="D5" s="42"/>
       <c r="E5" s="55"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="42"/>
-      <c r="B6" s="71"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="55"/>
       <c r="D6" s="42"/>
-      <c r="E6" s="71"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="36"/>
-      <c r="B7" s="55"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="55"/>
+      <c r="E6" s="55"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="36"/>
-      <c r="B8" s="55"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="55"/>
+      <c r="A8" s="36" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="36" t="s">
-        <v>119</v>
+      <c r="A10" s="40" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="40" t="s">
-        <v>86</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5">
+      <c r="A13" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="74"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="74" t="s">
+      <c r="A14" s="49"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="31.5">
-      <c r="A15" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="74"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="49"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>95</v>
-      </c>
+      <c r="A17" s="49"/>
+      <c r="B17" s="61"/>
+      <c r="E17" s="61"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="49"/>
+      <c r="B18" s="61"/>
+      <c r="E18" s="61"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="49"/>
@@ -1568,19 +1570,20 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="49"/>
-      <c r="B22" s="61"/>
-      <c r="E22" s="61"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="49"/>
-      <c r="B23" s="61"/>
-      <c r="E23" s="61"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="49"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="49"/>
+      <c r="A24" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="51" t="s">
@@ -1897,7 +1900,7 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="C48:C50"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>

<commit_message>
Added "autocomplete" to text input box for Species dropdown
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74FC77B-31B2-4464-A9F7-A7EEAF17F765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB33E29A-CB67-45D6-88B9-D8E00B8D15FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1560" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -1043,6 +1043,9 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1060,9 +1063,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1451,7 +1451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1506,42 +1506,52 @@
       <c r="E6" s="55"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="36" t="s">
-        <v>119</v>
-      </c>
+      <c r="A8" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5">
+      <c r="A9" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="75"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="40" t="s">
-        <v>86</v>
+      <c r="A10" s="49"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="74" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="31.5">
-      <c r="A13" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="74"/>
+      <c r="A12" s="49"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="49"/>
+      <c r="B13" s="61"/>
+      <c r="E13" s="61"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="49"/>
+      <c r="B14" s="61"/>
+      <c r="E14" s="61"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>95</v>
-      </c>
+      <c r="A15" s="49"/>
+      <c r="B15" s="61"/>
+      <c r="E15" s="61"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="49"/>
+      <c r="B16" s="61"/>
+      <c r="E16" s="61"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="49"/>
@@ -1550,29 +1560,27 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="49"/>
-      <c r="B18" s="61"/>
-      <c r="E18" s="61"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="49"/>
-      <c r="B19" s="61"/>
-      <c r="E19" s="61"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="49"/>
-      <c r="B20" s="61"/>
-      <c r="E20" s="61"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="49"/>
-      <c r="B21" s="61"/>
-      <c r="E21" s="61"/>
+      <c r="A20" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="49"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="49"/>
+      <c r="A22" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="51" t="s">
@@ -1597,7 +1605,7 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="73" t="s">
         <v>122</v>
       </c>
       <c r="B28" s="52"/>
@@ -1758,10 +1766,10 @@
       <c r="A48" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="75" t="s">
+      <c r="B48" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="76" t="s">
         <v>90</v>
       </c>
       <c r="E48" s="58"/>
@@ -1770,16 +1778,16 @@
       <c r="A49" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="73"/>
-      <c r="C49" s="75"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="76"/>
       <c r="E49" s="47"/>
     </row>
     <row r="50" spans="1:5" s="57" customFormat="1">
       <c r="A50" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="73"/>
-      <c r="C50" s="75"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="76"/>
       <c r="E50" s="47"/>
     </row>
     <row r="52" spans="1:5" ht="28.5">
@@ -1900,7 +1908,7 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="C48:C50"/>
   </mergeCells>
   <hyperlinks>
@@ -2272,13 +2280,13 @@
   <sheetData>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="18.75">
       <c r="A3" s="8"/>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="18.75">
       <c r="A4" s="9" t="s">
@@ -2469,7 +2477,7 @@
       <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -2477,7 +2485,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="77"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
@@ -2517,7 +2525,7 @@
       <c r="C20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="78" t="s">
+      <c r="E20" s="79" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2525,7 +2533,7 @@
       <c r="C21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="78"/>
+      <c r="E21" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update link text & links
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB33E29A-CB67-45D6-88B9-D8E00B8D15FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E044510-28A4-4C9B-8D64-D3CC064FEE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1560" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <author>Jim</author>
   </authors>
   <commentList>
-    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{29892D67-02C3-4457-AE65-66D16AC51274}">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>change the word Hauls to Sets in the Regions table, Sites table, and Sites popup</t>
-  </si>
-  <si>
-    <t>If a species is currently selected and SP panel is opened again, "Close" button has changed to "Go".  Still works to close panel, though.</t>
   </si>
   <si>
     <t>Put graphic object ID in hidden column?</t>
@@ -535,6 +532,15 @@
   </si>
   <si>
     <t>Prepare links for switching between SZ/FA/SS</t>
+  </si>
+  <si>
+    <t>Go/Close button</t>
+  </si>
+  <si>
+    <t>Sci. name ordering</t>
+  </si>
+  <si>
+    <t>concatenated DOI</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1052,10 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1092,13 +1098,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3247634</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>152264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1447,7 +1453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8762A0-C6E1-4E4F-887F-5F4A028E733F}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1477,54 +1483,52 @@
       <c r="E1" s="38"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="68" t="s">
-        <v>121</v>
-      </c>
+      <c r="A3" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="55"/>
       <c r="D3" s="42"/>
       <c r="E3" s="55"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="42"/>
-      <c r="B4" s="71"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="55"/>
       <c r="D4" s="42"/>
-      <c r="E4" s="71"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="36"/>
-      <c r="B5" s="55"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="55"/>
+      <c r="A5" s="40" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="36"/>
-      <c r="B6" s="55"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="55"/>
+      <c r="A6" s="49"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="74"/>
+      <c r="E7" s="74"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="75" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="31.5">
-      <c r="A9" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="75"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="74"/>
+      <c r="E8" s="74"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="49"/>
+      <c r="B9" s="74"/>
+      <c r="E9" s="74"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="49"/>
+      <c r="B10" s="74"/>
+      <c r="E10" s="74"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="41" t="s">
         <v>95</v>
@@ -1566,157 +1570,156 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="51"/>
+        <v>87</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>95</v>
+      </c>
       <c r="C20" s="51" t="s">
         <v>90</v>
       </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="49"/>
+      <c r="B21" s="36"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51" t="s">
-        <v>90</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B22" s="52"/>
+      <c r="C22" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="55"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="42"/>
+      <c r="B23" s="71"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="71"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="51" t="s">
-        <v>90</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B24" s="51"/>
       <c r="C24" s="51" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="73" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="55"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="36"/>
-      <c r="B29" s="55"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="55"/>
+      <c r="A28" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="52"/>
+      <c r="B30" s="52" t="s">
+        <v>90</v>
+      </c>
       <c r="C30" s="68" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="51" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="52"/>
+      <c r="C32" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="42"/>
+      <c r="E32" s="55"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="36"/>
+      <c r="B33" s="55"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="55"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="51"/>
-      <c r="E33" s="72" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="42"/>
-      <c r="B34" s="55"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="55"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="68" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="67" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="31.5">
-      <c r="A37" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="60"/>
-      <c r="C37" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="55"/>
+      <c r="A35" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="52"/>
+      <c r="C35" s="68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="52"/>
+      <c r="C37" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="51"/>
+      <c r="E37" s="72" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="60"/>
-      <c r="C38" s="67" t="s">
-        <v>90</v>
-      </c>
+      <c r="A38" s="42"/>
+      <c r="B38" s="55"/>
       <c r="D38" s="42"/>
       <c r="E38" s="55"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="42"/>
-      <c r="B39" s="55"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="55"/>
-    </row>
-    <row r="40" spans="1:5" s="63" customFormat="1">
-      <c r="A40" s="70" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="69"/>
-      <c r="C40" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="62"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="42"/>
-      <c r="B41" s="55"/>
+      <c r="A39" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="60"/>
+      <c r="C39" s="67" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="31.5">
+      <c r="A41" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="60"/>
+      <c r="C41" s="67" t="s">
+        <v>90</v>
+      </c>
       <c r="D41" s="42"/>
       <c r="E41" s="55"/>
     </row>
-    <row r="42" spans="1:5" ht="47.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="60"/>
+      <c r="C42" s="67" t="s">
         <v>90</v>
       </c>
       <c r="D42" s="42"/>
@@ -1728,16 +1731,15 @@
       <c r="D43" s="42"/>
       <c r="E43" s="55"/>
     </row>
-    <row r="44" spans="1:5" ht="94.5">
-      <c r="A44" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="56"/>
+    <row r="44" spans="1:5" s="63" customFormat="1">
+      <c r="A44" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="69"/>
       <c r="C44" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="D44" s="42"/>
-      <c r="E44" s="55"/>
+        <v>90</v>
+      </c>
+      <c r="D44" s="62"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="42"/>
@@ -1745,9 +1747,9 @@
       <c r="D45" s="42"/>
       <c r="E45" s="55"/>
     </row>
-    <row r="46" spans="1:5" ht="21" customHeight="1">
+    <row r="46" spans="1:5" ht="47.25">
       <c r="A46" s="46" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B46" s="56"/>
       <c r="C46" s="66" t="s">
@@ -1757,67 +1759,76 @@
       <c r="E46" s="55"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="36"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="55"/>
       <c r="D47" s="42"/>
       <c r="E47" s="55"/>
     </row>
-    <row r="48" spans="1:5" s="57" customFormat="1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="94.5">
       <c r="A48" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="56"/>
+      <c r="C48" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="42"/>
+      <c r="E48" s="55"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="42"/>
+      <c r="B49" s="55"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="55"/>
+    </row>
+    <row r="50" spans="1:5" ht="21" customHeight="1">
+      <c r="A50" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="56"/>
+      <c r="C50" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="42"/>
+      <c r="E50" s="55"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="36"/>
+      <c r="B51" s="55"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="55"/>
+    </row>
+    <row r="52" spans="1:5" s="57" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A52" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="76" t="s">
-        <v>90</v>
-      </c>
-      <c r="E48" s="58"/>
-    </row>
-    <row r="49" spans="1:5" s="57" customFormat="1">
-      <c r="A49" s="59" t="s">
+      <c r="B52" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" s="58"/>
+    </row>
+    <row r="53" spans="1:5" s="57" customFormat="1">
+      <c r="A53" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="74"/>
-      <c r="C49" s="76"/>
-      <c r="E49" s="47"/>
-    </row>
-    <row r="50" spans="1:5" s="57" customFormat="1">
-      <c r="A50" s="59" t="s">
+      <c r="B53" s="75"/>
+      <c r="C53" s="76"/>
+      <c r="E53" s="47"/>
+    </row>
+    <row r="54" spans="1:5" s="57" customFormat="1">
+      <c r="A54" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="74"/>
-      <c r="C50" s="76"/>
-      <c r="E50" s="47"/>
-    </row>
-    <row r="52" spans="1:5" ht="28.5">
-      <c r="A52" s="54" t="s">
+      <c r="B54" s="75"/>
+      <c r="C54" s="76"/>
+      <c r="E54" s="47"/>
+    </row>
+    <row r="56" spans="1:5" ht="28.5">
+      <c r="A56" s="54" t="s">
         <v>94</v>
-      </c>
-      <c r="B52" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="28.5">
-      <c r="A54" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="B54" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="45"/>
-    </row>
-    <row r="56" spans="1:5" ht="42.75">
-      <c r="A56" s="54" t="s">
-        <v>92</v>
       </c>
       <c r="B56" s="52" t="s">
         <v>95</v>
@@ -1826,73 +1837,86 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="45"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="51" t="s">
+    <row r="58" spans="1:5" ht="28.5">
+      <c r="A58" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="45"/>
+    </row>
+    <row r="60" spans="1:5" ht="42.75">
+      <c r="A60" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="45"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="53" t="s">
+      <c r="B62" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C62" s="68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="B60" s="52"/>
-      <c r="C60" s="68" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="46" t="s">
+      <c r="B64" s="52"/>
+      <c r="C64" s="68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62" s="66" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="48" t="s">
+      <c r="B66" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C66" s="66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C64" s="66" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="31.5">
-      <c r="A66" s="46" t="s">
+      <c r="B68" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="31.5">
+      <c r="A70" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C66" s="66" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="43"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="43"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="43"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="43"/>
+      <c r="B70" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70" s="66" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="43"/>
@@ -1901,18 +1925,29 @@
       <c r="A75" s="43"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="44" t="s">
+      <c r="A76" s="43"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="43"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="43"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="43"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="44" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C48:C50"/>
+  <mergeCells count="2">
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A64" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
+    <hyperlink ref="A68" r:id="rId1" xr:uid="{5B747565-554E-A24E-8BB4-ED8F3C3E88AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>

</xml_diff>

<commit_message>
Species dropdown ordering by Scientific Name, web.config requires reload after 10 minutes
</commit_message>
<xml_diff>
--- a/Docs/SZ JS site issues.xlsx
+++ b/Docs/SZ JS site issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SZdev\SZ_JS_4x\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E044510-28A4-4C9B-8D64-D3CC064FEE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0330B6EA-97B8-4BDC-8EE4-06DAD61FC834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1560" windowWidth="27420" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="125">
   <si>
     <t>identify areas that could be debugged by Tristan?</t>
   </si>
@@ -1457,7 +1457,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1497,17 +1497,19 @@
       <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="40" t="s">
-        <v>123</v>
-      </c>
+      <c r="A5" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="74"/>
+      <c r="E5" s="74"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="49"/>
+      <c r="B6" s="74"/>
+      <c r="E6" s="74"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="50" t="s">
-        <v>124</v>
-      </c>
+      <c r="A7" s="49"/>
       <c r="B7" s="74"/>
       <c r="E7" s="74"/>
     </row>
@@ -1517,25 +1519,25 @@
       <c r="E8" s="74"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="49"/>
-      <c r="B9" s="74"/>
-      <c r="E9" s="74"/>
+      <c r="A9" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="49"/>
-      <c r="B10" s="74"/>
-      <c r="E10" s="74"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>95</v>
-      </c>
+      <c r="A11" s="49"/>
+      <c r="B11" s="61"/>
+      <c r="E11" s="61"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="49"/>
+      <c r="B12" s="61"/>
+      <c r="E12" s="61"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="49"/>
@@ -1554,20 +1556,19 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="49"/>
-      <c r="B16" s="61"/>
-      <c r="E16" s="61"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="49"/>
-      <c r="B17" s="61"/>
-      <c r="E17" s="61"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="49"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="49"/>
-    </row>
+    </row>
+    <row r="18" spans="1:5" s="51" customFormat="1">
+      <c r="A18" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="51" customFormat="1"/>
     <row r="20" spans="1:5">
       <c r="A20" s="51" t="s">
         <v>87</v>

</xml_diff>